<commit_message>
Commiting thr final assignment
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdi/OneDrive - Deloitte (O365D)/Documents/Selenium_Main_Assignmnt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9072C60-29CB-C248-BAEA-00D2A0F4DEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CEB8ED-EE7E-C24E-BC24-5B6BEE641386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>